<commit_message>
Fixed template and a few others
</commit_message>
<xml_diff>
--- a/DibsOrderMgmt/HiveTemplates/HIVE_PublisherPO_Template.xlsx
+++ b/DibsOrderMgmt/HiveTemplates/HIVE_PublisherPO_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\MEP - Shared\BrainHive\BH_OrderMgmt\HIVE_Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RickyHarlow\source\repos\DibsOrderMgmt\DibsOrderMgmt\HiveTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2997D725-69B3-4983-9713-92BA30282B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E41BD4-D397-4C9E-BF4A-029A7128C0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="240">
   <si>
-    <t xml:space="preserve">BRAIN HIVE INVOICE  </t>
-  </si>
-  <si>
     <t>Brain Hive Order Form</t>
   </si>
   <si>
@@ -771,6 +768,9 @@
   </si>
   <si>
     <t>919.395.7315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAIN HIVE PURCHASE ORDER  </t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1189,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1408,6 +1407,15 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1438,6 +1446,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1447,17 +1458,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1508,15 +1510,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>73660</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>154940</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1539,8 +1541,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73898" y="95250"/>
-          <a:ext cx="1274842" cy="712314"/>
+          <a:off x="0" y="38100"/>
+          <a:ext cx="1278890" cy="723900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1558,7 +1560,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1307465</xdr:colOff>
+      <xdr:colOff>1412240</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>120015</xdr:rowOff>
     </xdr:to>
@@ -1894,38 +1896,39 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.375" customWidth="1"/>
-    <col min="3" max="3" width="5.375" customWidth="1"/>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
     <col min="4" max="4" width="9.375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="19.625" customWidth="1"/>
     <col min="6" max="6" width="8.875" customWidth="1"/>
     <col min="7" max="7" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="14.625" style="86" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="85" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="98" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="114" t="s">
-        <v>1</v>
+      <c r="C1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="100" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -1940,359 +1943,359 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="87"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="88"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="17" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="B6" s="97"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="98"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="20" t="s">
+      <c r="F6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22"/>
-    </row>
-    <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="108" t="s">
+      <c r="B7" s="110"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="104"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="110"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="104"/>
+    </row>
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="110"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="106"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="111"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="106"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="111" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="111"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="102"/>
-    </row>
-    <row r="8" spans="1:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="102"/>
-    </row>
-    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="104"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="104"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="115" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="115"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="105" t="s">
+      <c r="G12" s="108"/>
+      <c r="H12" s="109"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="78"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="88"/>
+      <c r="B14" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="90"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="92"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="106"/>
-      <c r="H12" s="107"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="89"/>
-      <c r="B14" s="90" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="91"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="93"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="30" t="s">
+      <c r="F15" s="29"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="30" t="s">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="31" t="str">
+      <c r="B16" s="30" t="str">
         <f>B3</f>
         <v>8/3/2021</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="30" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="32" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="C17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="D17" s="34"/>
+      <c r="E17" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36" t="s">
+      <c r="F17" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="G17" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="80" t="s">
+      <c r="H17" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="87" t="s">
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="B18" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="C18" s="38">
+        <v>1</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="39">
-        <v>1</v>
-      </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="42">
+      <c r="F18" s="41">
         <v>0.65</v>
       </c>
-      <c r="G18" s="81"/>
-      <c r="H18" s="43">
+      <c r="G18" s="80"/>
+      <c r="H18" s="42">
         <f>G18*C18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="43"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="42"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="52"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="53">
+      <c r="A20" s="47"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="52">
         <f>SUM(H18:H18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="55"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="54"/>
     </row>
     <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="58"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="57"/>
     </row>
     <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="58"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="57"/>
     </row>
     <row r="24" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="48"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="58">
+      <c r="A24" s="47"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="56"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="57">
         <f>SUM(H20:H23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="109" t="s">
+      <c r="A25" s="112" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="112"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="84"/>
+    </row>
+    <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="113" t="s">
         <v>236</v>
       </c>
-      <c r="B25" s="109"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="85"/>
-    </row>
-    <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="110" t="s">
+      <c r="B26" s="114"/>
+      <c r="E26" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="E26" s="74" t="s">
+      <c r="G26" s="114" t="s">
         <v>238</v>
       </c>
-      <c r="G26" s="111" t="s">
+      <c r="H26" s="114"/>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="98" t="s">
         <v>239</v>
       </c>
-      <c r="H26" s="111"/>
-    </row>
-    <row r="27" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="112" t="s">
+      <c r="B27" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="113"/>
-      <c r="G27" s="113"/>
-      <c r="H27" s="113" t="s">
-        <v>1</v>
+      <c r="C27" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="99"/>
+      <c r="E27" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="99"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="100" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="99"/>
-      <c r="B28" s="100"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100"/>
+      <c r="A28" s="101"/>
+      <c r="B28" s="102"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="102"/>
+      <c r="E28" s="102"/>
+      <c r="F28" s="102"/>
+      <c r="G28" s="102"/>
+      <c r="H28" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2332,1382 +2335,1382 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.375" style="59" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="58" customWidth="1"/>
     <col min="2" max="2" width="36.875" customWidth="1"/>
-    <col min="3" max="3" width="10.625" style="60"/>
+    <col min="3" max="3" width="10.625" style="59"/>
     <col min="4" max="4" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="60" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="58">
+        <v>9781618102348</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="59">
-        <v>9781618102348</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="58">
+        <v>9781621698005</v>
+      </c>
+      <c r="B5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="59">
-        <v>9781621698005</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="58">
+        <v>9781681917795</v>
+      </c>
+      <c r="B6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="59">
-        <v>9781681917795</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="58">
+        <v>9781681918150</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="59">
-        <v>9781681918150</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="58">
+        <v>9781683424345</v>
+      </c>
+      <c r="B8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="59">
-        <v>9781683424345</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="58">
+        <v>9781683424468</v>
+      </c>
+      <c r="B9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="59">
-        <v>9781683424468</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="58">
+        <v>9781643690773</v>
+      </c>
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="59">
-        <v>9781643690773</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="58">
+        <v>9781731612281</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="59">
-        <v>9781731612281</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="58">
+        <v>9781618102232</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="59">
-        <v>9781618102232</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="58">
+        <v>9781627178631</v>
+      </c>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="59">
-        <v>9781627178631</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="58">
+        <v>9781681917887</v>
+      </c>
+      <c r="B16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="59">
-        <v>9781681917887</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="58">
+        <v>9781681918129</v>
+      </c>
+      <c r="B17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="59">
-        <v>9781681918129</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="58">
+        <v>9781681918617</v>
+      </c>
+      <c r="B18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="59">
-        <v>9781681918617</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="58">
+        <v>9781683424437</v>
+      </c>
+      <c r="B19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="59">
-        <v>9781683424437</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="58">
+        <v>9781643691107</v>
+      </c>
+      <c r="B20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="59">
-        <v>9781643691107</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C20" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="58">
+        <v>9781731612335</v>
+      </c>
+      <c r="B21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="59">
-        <v>9781731612335</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="58">
+        <v>9781618102317</v>
+      </c>
+      <c r="B24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="59">
-        <v>9781618102317</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="D24" t="s">
         <v>72</v>
       </c>
-      <c r="D24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="58">
+        <v>9781618102416</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="59">
-        <v>9781618102416</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C25" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="58">
+        <v>9781634300711</v>
+      </c>
+      <c r="B26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="59">
-        <v>9781634300711</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="58">
+        <v>9781634304979</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="59">
-        <v>9781634304979</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="58">
+        <v>9781681918655</v>
+      </c>
+      <c r="B28" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="59">
-        <v>9781681918655</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C28" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="58">
+        <v>9781683424505</v>
+      </c>
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="59">
-        <v>9781683424505</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C29" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="58">
+        <v>9781641566469</v>
+      </c>
+      <c r="B30" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="59">
-        <v>9781641566469</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C30" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="58">
+        <v>9781641566087</v>
+      </c>
+      <c r="B31" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="59">
-        <v>9781641566087</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C31" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="58">
+        <v>9781634300759</v>
+      </c>
+      <c r="B34" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="59">
-        <v>9781634300759</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C34" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="60" t="s">
+      <c r="D34" t="s">
         <v>89</v>
       </c>
-      <c r="D34" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="58">
+        <v>9781634304900</v>
+      </c>
+      <c r="B35" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="59">
-        <v>9781634304900</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C35" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="58">
+        <v>9781634304986</v>
+      </c>
+      <c r="B36" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="59">
-        <v>9781634304986</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C36" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="58">
+        <v>9781681917801</v>
+      </c>
+      <c r="B37" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="59">
-        <v>9781681917801</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C37" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="58">
+        <v>9781683424512</v>
+      </c>
+      <c r="B38" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="59">
-        <v>9781683424512</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C38" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="58">
+        <v>9781683424420</v>
+      </c>
+      <c r="B39" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="59">
-        <v>9781683424420</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C39" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="58">
+        <v>9781641566049</v>
+      </c>
+      <c r="B40" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="59">
-        <v>9781641566049</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C40" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="58">
+        <v>9781643690711</v>
+      </c>
+      <c r="B41" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="59">
-        <v>9781643690711</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C41" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="58">
+        <v>9781615905584</v>
+      </c>
+      <c r="B44" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="59">
-        <v>9781615905584</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C44" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="D44" t="s">
         <v>106</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="58">
+        <v>9781618102393</v>
+      </c>
+      <c r="B45" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="59">
-        <v>9781618102393</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C45" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="58">
+        <v>9781634304924</v>
+      </c>
+      <c r="B46" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="59">
-        <v>9781634304924</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C46" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="58">
+        <v>9781683424499</v>
+      </c>
+      <c r="B47" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="59">
-        <v>9781683424499</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C47" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="58">
+        <v>9781683424482</v>
+      </c>
+      <c r="B48" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="59">
-        <v>9781683424482</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C48" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" t="s">
         <v>114</v>
       </c>
-      <c r="C48" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="58">
+        <v>9781641565325</v>
+      </c>
+      <c r="B49" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="59">
-        <v>9781641565325</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C49" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="58">
+        <v>9781641565363</v>
+      </c>
+      <c r="B50" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="59">
-        <v>9781641565363</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C50" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="58">
+        <v>9781643691015</v>
+      </c>
+      <c r="B51" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="59">
-        <v>9781643691015</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C51" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="58">
+        <v>9781618102577</v>
+      </c>
+      <c r="B54" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="59">
-        <v>9781618102577</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C54" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="60" t="s">
+      <c r="D54" t="s">
         <v>123</v>
       </c>
-      <c r="D54" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="58">
+        <v>9781627178686</v>
+      </c>
+      <c r="B55" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="59">
-        <v>9781627178686</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C55" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" t="s">
         <v>125</v>
       </c>
-      <c r="C55" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="58">
+        <v>9781641565417</v>
+      </c>
+      <c r="B56" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="59">
-        <v>9781641565417</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C56" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" t="s">
         <v>127</v>
       </c>
-      <c r="C56" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="58">
+        <v>9781641565783</v>
+      </c>
+      <c r="B57" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="59">
-        <v>9781641565783</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C57" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D57" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D57" t="s">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="58">
+        <v>9781641565745</v>
+      </c>
+      <c r="B58" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="59">
-        <v>9781641565745</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C58" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" t="s">
         <v>131</v>
       </c>
-      <c r="C58" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D58" t="s">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="58">
+        <v>9781643690704</v>
+      </c>
+      <c r="B59" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="59">
-        <v>9781643690704</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C59" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D59" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D59" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="58">
+        <v>9781643690902</v>
+      </c>
+      <c r="B60" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="59">
-        <v>9781643690902</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C60" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" t="s">
         <v>135</v>
       </c>
-      <c r="C60" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D60" t="s">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="58">
+        <v>9781643691152</v>
+      </c>
+      <c r="B61" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="59">
-        <v>9781643691152</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C61" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" t="s">
         <v>137</v>
       </c>
-      <c r="C61" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="58">
+        <v>9781606947043</v>
+      </c>
+      <c r="B64" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="59">
-        <v>9781606947043</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C64" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="C64" s="60" t="s">
+      <c r="D64" t="s">
         <v>140</v>
       </c>
-      <c r="D64" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="58">
+        <v>9781606945285</v>
+      </c>
+      <c r="B65" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="59">
-        <v>9781606945285</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C65" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" t="s">
         <v>142</v>
       </c>
-      <c r="C65" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="D65" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="58">
+        <v>9781606945315</v>
+      </c>
+      <c r="B66" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="59">
-        <v>9781606945315</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="C66" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D66" t="s">
         <v>144</v>
       </c>
-      <c r="C66" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="D66" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="58">
+        <v>9781612362328</v>
+      </c>
+      <c r="B67" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="59">
-        <v>9781612362328</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="C67" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" t="s">
         <v>146</v>
       </c>
-      <c r="C67" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="D67" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="58">
+        <v>9781681914268</v>
+      </c>
+      <c r="B68" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="59">
-        <v>9781681914268</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="C68" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" t="s">
         <v>148</v>
       </c>
-      <c r="C68" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="D68" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="58">
+        <v>9781681918723</v>
+      </c>
+      <c r="B69" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="59">
-        <v>9781681918723</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C69" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" t="s">
         <v>150</v>
       </c>
-      <c r="C69" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="D69" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="58">
+        <v>9781641565981</v>
+      </c>
+      <c r="B70" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="59">
-        <v>9781641565981</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="C70" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" t="s">
         <v>152</v>
       </c>
-      <c r="C70" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="D70" t="s">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="58">
+        <v>9781643691114</v>
+      </c>
+      <c r="B71" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="59">
-        <v>9781643691114</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="C71" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D71" t="s">
         <v>154</v>
       </c>
-      <c r="C71" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="D71" t="s">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="58">
+        <v>9781617419874</v>
+      </c>
+      <c r="B74" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="59">
-        <v>9781617419874</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C74" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="C74" s="60" t="s">
+      <c r="D74" t="s">
         <v>157</v>
       </c>
-      <c r="D74" t="s">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="58">
+        <v>9781618102539</v>
+      </c>
+      <c r="B75" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="59">
-        <v>9781618102539</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="C75" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" t="s">
         <v>159</v>
       </c>
-      <c r="C75" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D75" t="s">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="58">
+        <v>9781681917962</v>
+      </c>
+      <c r="B76" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="59">
-        <v>9781681917962</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C76" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" t="s">
         <v>161</v>
       </c>
-      <c r="C76" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D76" t="s">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="58">
+        <v>9781681918433</v>
+      </c>
+      <c r="B77" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="59">
-        <v>9781681918433</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="C77" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" t="s">
         <v>163</v>
       </c>
-      <c r="C77" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77" t="s">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="58">
+        <v>9781681918648</v>
+      </c>
+      <c r="B78" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="59">
-        <v>9781681918648</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="C78" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D78" t="s">
         <v>165</v>
       </c>
-      <c r="C78" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D78" t="s">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="58">
+        <v>9781641565424</v>
+      </c>
+      <c r="B79" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="59">
-        <v>9781641565424</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="C79" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" t="s">
         <v>167</v>
       </c>
-      <c r="C79" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D79" t="s">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="58">
+        <v>9781643691138</v>
+      </c>
+      <c r="B80" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="59">
-        <v>9781643691138</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="C80" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D80" t="s">
         <v>169</v>
       </c>
-      <c r="C80" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D80" t="s">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="58">
+        <v>9781643691022</v>
+      </c>
+      <c r="B81" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="59">
-        <v>9781643691022</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="C81" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D81" t="s">
         <v>171</v>
       </c>
-      <c r="C81" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="D81" t="s">
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="58">
+        <v>9781681914329</v>
+      </c>
+      <c r="B84" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="59">
-        <v>9781681914329</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="C84" s="59" t="s">
         <v>173</v>
       </c>
-      <c r="C84" s="60" t="s">
+      <c r="D84" t="s">
         <v>174</v>
       </c>
-      <c r="D84" t="s">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="58">
+        <v>9781681914312</v>
+      </c>
+      <c r="B85" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="59">
-        <v>9781681914312</v>
-      </c>
-      <c r="B85" t="s">
+      <c r="C85" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D85" t="s">
         <v>176</v>
       </c>
-      <c r="C85" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D85" t="s">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="58">
+        <v>9781681914343</v>
+      </c>
+      <c r="B86" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="59">
-        <v>9781681914343</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="C86" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D86" t="s">
         <v>178</v>
       </c>
-      <c r="C86" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D86" t="s">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="58">
+        <v>9781681914428</v>
+      </c>
+      <c r="B87" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="59">
-        <v>9781681914428</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="C87" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D87" t="s">
         <v>180</v>
       </c>
-      <c r="C87" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D87" t="s">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="58">
+        <v>9781641565806</v>
+      </c>
+      <c r="B88" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="59">
-        <v>9781641565806</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C88" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D88" t="s">
         <v>182</v>
       </c>
-      <c r="C88" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D88" t="s">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="58">
+        <v>9781641565813</v>
+      </c>
+      <c r="B89" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="59">
-        <v>9781641565813</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="C89" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D89" t="s">
         <v>184</v>
       </c>
-      <c r="C89" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D89" t="s">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="58">
+        <v>9781641565622</v>
+      </c>
+      <c r="B90" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="59">
-        <v>9781641565622</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="C90" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D90" t="s">
         <v>186</v>
       </c>
-      <c r="C90" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D90" t="s">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="58">
+        <v>9781641566186</v>
+      </c>
+      <c r="B91" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="59">
-        <v>9781641566186</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C91" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D91" t="s">
         <v>188</v>
       </c>
-      <c r="C91" s="60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D91" t="s">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="58">
+        <v>9781618102560</v>
+      </c>
+      <c r="B94" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="59">
-        <v>9781618102560</v>
-      </c>
-      <c r="B94" t="s">
+      <c r="C94" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="C94" s="60" t="s">
+      <c r="D94" t="s">
         <v>191</v>
       </c>
-      <c r="D94" t="s">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="58">
+        <v>9781641565431</v>
+      </c>
+      <c r="B95" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="59">
-        <v>9781641565431</v>
-      </c>
-      <c r="B95" t="s">
+      <c r="C95" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D95" t="s">
         <v>193</v>
       </c>
-      <c r="C95" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D95" t="s">
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="58">
+        <v>9781641565820</v>
+      </c>
+      <c r="B96" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="59">
-        <v>9781641565820</v>
-      </c>
-      <c r="B96" t="s">
+      <c r="C96" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D96" t="s">
         <v>195</v>
       </c>
-      <c r="C96" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D96" t="s">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="58">
+        <v>9781641565646</v>
+      </c>
+      <c r="B97" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="59">
-        <v>9781641565646</v>
-      </c>
-      <c r="B97" t="s">
+      <c r="C97" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D97" t="s">
         <v>197</v>
       </c>
-      <c r="C97" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D97" t="s">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="58">
+        <v>9781641565615</v>
+      </c>
+      <c r="B98" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="59">
-        <v>9781641565615</v>
-      </c>
-      <c r="B98" t="s">
+      <c r="C98" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D98" t="s">
         <v>199</v>
       </c>
-      <c r="C98" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D98" t="s">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="58">
+        <v>9781641565592</v>
+      </c>
+      <c r="B99" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="59">
-        <v>9781641565592</v>
-      </c>
-      <c r="B99" t="s">
+      <c r="C99" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D99" t="s">
         <v>201</v>
       </c>
-      <c r="C99" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D99" t="s">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="58">
+        <v>9781641566179</v>
+      </c>
+      <c r="B100" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="59">
-        <v>9781641566179</v>
-      </c>
-      <c r="B100" t="s">
+      <c r="C100" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D100" t="s">
         <v>203</v>
       </c>
-      <c r="C100" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D100" t="s">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="58">
+        <v>9781643690759</v>
+      </c>
+      <c r="B101" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="59">
-        <v>9781643690759</v>
-      </c>
-      <c r="B101" t="s">
+      <c r="C101" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D101" t="s">
         <v>205</v>
       </c>
-      <c r="C101" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D101" t="s">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="58">
+        <v>9781618102546</v>
+      </c>
+      <c r="B104" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="59">
-        <v>9781618102546</v>
-      </c>
-      <c r="B104" t="s">
+      <c r="C104" s="59" t="s">
         <v>207</v>
       </c>
-      <c r="C104" s="60" t="s">
+      <c r="D104" t="s">
         <v>208</v>
       </c>
-      <c r="D104" t="s">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="58">
+        <v>9781681914404</v>
+      </c>
+      <c r="B105" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="59">
-        <v>9781681914404</v>
-      </c>
-      <c r="B105" t="s">
+      <c r="C105" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="D105" t="s">
         <v>210</v>
       </c>
-      <c r="C105" s="60" t="s">
-        <v>208</v>
-      </c>
-      <c r="D105" t="s">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="58">
+        <v>9781641565608</v>
+      </c>
+      <c r="B106" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="59">
-        <v>9781641565608</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="C106" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="D106" t="s">
         <v>212</v>
       </c>
-      <c r="C106" s="60" t="s">
-        <v>208</v>
-      </c>
-      <c r="D106" t="s">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="63">
+        <v>9781641565462</v>
+      </c>
+      <c r="B107" s="64" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="64">
-        <v>9781641565462</v>
-      </c>
-      <c r="B107" s="65" t="s">
+      <c r="C107" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="C107" s="60" t="s">
+      <c r="D107" t="s">
         <v>215</v>
       </c>
-      <c r="D107" t="s">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="58">
+        <v>9781681914237</v>
+      </c>
+      <c r="B108" s="65" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="59">
-        <v>9781681914237</v>
-      </c>
-      <c r="B108" s="66" t="s">
+      <c r="C108" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D108" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="66">
+        <v>9781731612823</v>
+      </c>
+      <c r="B109" s="67" t="s">
         <v>217</v>
       </c>
-      <c r="C108" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D108" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="67">
-        <v>9781731612823</v>
-      </c>
-      <c r="B109" s="68" t="s">
+      <c r="C109" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="D109" t="s">
         <v>218</v>
       </c>
-      <c r="C109" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="D109" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="58">
+        <v>9781641565639</v>
+      </c>
+      <c r="B110" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="59">
+      <c r="C110" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D110" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="66">
+        <v>9781731612946</v>
+      </c>
+      <c r="B111" s="67" t="s">
+        <v>221</v>
+      </c>
+      <c r="C111" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D111" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="68"/>
+      <c r="B112" s="67"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="66">
+        <v>9781731612984</v>
+      </c>
+      <c r="B113" s="67" t="s">
+        <v>223</v>
+      </c>
+      <c r="C113" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D113" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="66">
+        <v>9781731612939</v>
+      </c>
+      <c r="B114" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="C114" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D114" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="66">
+        <v>9781731612946</v>
+      </c>
+      <c r="B115" s="67" t="s">
+        <v>221</v>
+      </c>
+      <c r="C115" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D115" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="66">
+        <v>9781731612816</v>
+      </c>
+      <c r="B116" s="67" t="s">
+        <v>227</v>
+      </c>
+      <c r="C116" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D116" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="66">
+        <v>9781731612793</v>
+      </c>
+      <c r="B117" s="67" t="s">
+        <v>229</v>
+      </c>
+      <c r="C117" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D117" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="58">
+        <v>9781641565851</v>
+      </c>
+      <c r="B118" t="s">
+        <v>231</v>
+      </c>
+      <c r="C118" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D118" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="58">
         <v>9781641565639</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B119" t="s">
+        <v>219</v>
+      </c>
+      <c r="C119" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D119" t="s">
         <v>220</v>
       </c>
-      <c r="C110" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D110" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="67">
-        <v>9781731612946</v>
-      </c>
-      <c r="B111" s="68" t="s">
-        <v>222</v>
-      </c>
-      <c r="C111" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D111" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="69"/>
-      <c r="B112" s="68"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="67">
-        <v>9781731612984</v>
-      </c>
-      <c r="B113" s="68" t="s">
-        <v>224</v>
-      </c>
-      <c r="C113" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D113" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="67">
-        <v>9781731612939</v>
-      </c>
-      <c r="B114" s="68" t="s">
-        <v>226</v>
-      </c>
-      <c r="C114" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D114" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="67">
-        <v>9781731612946</v>
-      </c>
-      <c r="B115" s="68" t="s">
-        <v>222</v>
-      </c>
-      <c r="C115" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D115" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="67">
-        <v>9781731612816</v>
-      </c>
-      <c r="B116" s="68" t="s">
-        <v>228</v>
-      </c>
-      <c r="C116" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D116" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="67">
-        <v>9781731612793</v>
-      </c>
-      <c r="B117" s="68" t="s">
-        <v>230</v>
-      </c>
-      <c r="C117" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D117" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="59">
-        <v>9781641565851</v>
-      </c>
-      <c r="B118" t="s">
-        <v>232</v>
-      </c>
-      <c r="C118" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D118" t="s">
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="58">
+        <v>9781641566155</v>
+      </c>
+      <c r="B120" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="59">
-        <v>9781641565639</v>
-      </c>
-      <c r="B119" t="s">
-        <v>220</v>
-      </c>
-      <c r="C119" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D119" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="59">
-        <v>9781641566155</v>
-      </c>
-      <c r="B120" t="s">
+      <c r="C120" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="D120" t="s">
         <v>234</v>
-      </c>
-      <c r="C120" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="D120" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>